<commit_message>
Finished the prisoner class.
- Added new ability for the class specials to reduce enemy stats and
  increase spell evasion.
</commit_message>
<xml_diff>
--- a/resources/data-imports/celestials.xlsx
+++ b/resources/data-imports/celestials.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>id</t>
   </si>
@@ -131,7 +131,7 @@
     <t>counter_resistance</t>
   </si>
   <si>
-    <t>quest_item_id</t>
+    <t>quest_item_name</t>
   </si>
   <si>
     <t>quest_item_drop_chance</t>
@@ -143,235 +143,148 @@
     <t>celestial_type</t>
   </si>
   <si>
+    <t>Sinister Liar</t>
+  </si>
+  <si>
+    <t>150000-160000</t>
+  </si>
+  <si>
+    <t>Dungeon Ink</t>
+  </si>
+  <si>
+    <t>Corrupted Plane Walker</t>
+  </si>
+  <si>
+    <t>170000-180000</t>
+  </si>
+  <si>
+    <t>Shadow of the Depths</t>
+  </si>
+  <si>
+    <t>190000-200000</t>
+  </si>
+  <si>
+    <t>Angelic Soldier</t>
+  </si>
+  <si>
+    <t>210000-240000</t>
+  </si>
+  <si>
+    <t>Red Raging Treasure Mage</t>
+  </si>
+  <si>
+    <t>240000-260000</t>
+  </si>
+  <si>
+    <t>King of the Duegar</t>
+  </si>
+  <si>
+    <t>290000-300000</t>
+  </si>
+  <si>
     <t>Celestial Treasure Goblin</t>
   </si>
   <si>
-    <t>50000-70000</t>
-  </si>
-  <si>
-    <t>50000-70001</t>
+    <t>100000-125000</t>
+  </si>
+  <si>
+    <t>Alchemist Tools</t>
   </si>
   <si>
     <t>Faceless Shadow</t>
   </si>
   <si>
-    <t>60000-80000</t>
-  </si>
-  <si>
-    <t>60000-80001</t>
-  </si>
-  <si>
-    <t>Sinister Liar</t>
-  </si>
-  <si>
-    <t>70000-95000</t>
-  </si>
-  <si>
-    <t>70000-95001</t>
-  </si>
-  <si>
-    <t>Corrupted Plane Walker</t>
-  </si>
-  <si>
-    <t>120000-140000</t>
-  </si>
-  <si>
-    <t>120000-140001</t>
-  </si>
-  <si>
-    <t>Shadow of the Depths</t>
-  </si>
-  <si>
-    <t>160000-180000</t>
-  </si>
-  <si>
-    <t>160000-180001</t>
-  </si>
-  <si>
-    <t>Angelic Soldier</t>
-  </si>
-  <si>
-    <t>190000-230000</t>
-  </si>
-  <si>
-    <t>190000-230001</t>
-  </si>
-  <si>
-    <t>Red Raging Treasure Mage</t>
-  </si>
-  <si>
-    <t>240000-260000</t>
-  </si>
-  <si>
-    <t>240000-260001</t>
-  </si>
-  <si>
-    <t>King of the Duegar</t>
-  </si>
-  <si>
-    <t>290000-299999</t>
+    <t>130000-140000</t>
+  </si>
+  <si>
+    <t>Winged Baby Doll</t>
   </si>
   <si>
     <t>Death Eater</t>
   </si>
   <si>
-    <t>280000-300000</t>
-  </si>
-  <si>
-    <t>280000-300001</t>
-  </si>
-  <si>
     <t>Labyrinth Hellraiser</t>
   </si>
   <si>
-    <t>340000-360000</t>
-  </si>
-  <si>
-    <t>340000-360001</t>
-  </si>
-  <si>
     <t>Witch's Pet</t>
   </si>
   <si>
-    <t>380000-420000</t>
-  </si>
-  <si>
-    <t>380000-420001</t>
+    <t>River Styx Sandals</t>
   </si>
   <si>
     <t>Minotaur God</t>
   </si>
   <si>
-    <t>440000-480000</t>
-  </si>
-  <si>
-    <t>440000-480001</t>
-  </si>
-  <si>
-    <t>Winged Baby Doll</t>
-  </si>
-  <si>
-    <t>490000-510000</t>
-  </si>
-  <si>
-    <t>490000-510001</t>
-  </si>
-  <si>
     <t>Labyrinth Alchemizer</t>
   </si>
   <si>
-    <t>530000-560000</t>
-  </si>
-  <si>
-    <t>530000-560001</t>
+    <t>Hell Dragon of Kazard</t>
+  </si>
+  <si>
+    <t>Godless Wizard</t>
+  </si>
+  <si>
+    <t>Fanatic of Tlessa</t>
+  </si>
+  <si>
+    <t>Githzerai Monk of Labyrinth</t>
+  </si>
+  <si>
+    <t>310000-400000</t>
   </si>
   <si>
     <t>Trained Angelic Swordsmen</t>
   </si>
   <si>
-    <t>575000-625000</t>
-  </si>
-  <si>
-    <t>575000-625001</t>
-  </si>
-  <si>
-    <t>Hell Dragon of Kazard</t>
-  </si>
-  <si>
-    <t>630000-650000</t>
-  </si>
-  <si>
-    <t>630000-650001</t>
-  </si>
-  <si>
-    <t>Godless Wizard</t>
-  </si>
-  <si>
-    <t>666000-690000</t>
-  </si>
-  <si>
-    <t>666000-690001</t>
-  </si>
-  <si>
-    <t>Fanatic of Tlessa</t>
-  </si>
-  <si>
-    <t>700000-740000</t>
-  </si>
-  <si>
-    <t>700000-740001</t>
-  </si>
-  <si>
     <t>Slave Trader</t>
   </si>
   <si>
-    <t>760000-800000</t>
-  </si>
-  <si>
-    <t>760000-800001</t>
-  </si>
-  <si>
     <t>Pirate Lord</t>
   </si>
   <si>
-    <t>820000-840000</t>
-  </si>
-  <si>
-    <t>820000-840001</t>
-  </si>
-  <si>
     <t>Hell God</t>
   </si>
   <si>
-    <t>860000-900000</t>
-  </si>
-  <si>
-    <t>860000-900001</t>
-  </si>
-  <si>
     <t>Archangel Kalix</t>
   </si>
   <si>
-    <t>910000-940000</t>
-  </si>
-  <si>
-    <t>910000-940001</t>
-  </si>
-  <si>
     <t>The Child</t>
   </si>
   <si>
-    <t>960000-980000</t>
-  </si>
-  <si>
-    <t>960000-980001</t>
-  </si>
-  <si>
-    <t>Beholder of the Depths</t>
-  </si>
-  <si>
-    <t>990000-999999</t>
-  </si>
-  <si>
-    <t>990000-1000000</t>
+    <t>275000-325000</t>
+  </si>
+  <si>
+    <t>Lord of the Storm Giants</t>
+  </si>
+  <si>
+    <t>405000-450000</t>
   </si>
   <si>
     <t>Shadow Fang Wolf</t>
   </si>
   <si>
-    <t>1200000-1300000</t>
-  </si>
-  <si>
-    <t>1200000-1300001</t>
+    <t>75000-120000</t>
+  </si>
+  <si>
+    <t>Satanic Sigil</t>
   </si>
   <si>
     <t>Haunted Aberration</t>
   </si>
   <si>
-    <t>1400000-1600000</t>
-  </si>
-  <si>
-    <t>1400000-1600001</t>
+    <t>125000-150000</t>
+  </si>
+  <si>
+    <t>370000-390000</t>
+  </si>
+  <si>
+    <t>Magician's Enchanted Copper Coin</t>
+  </si>
+  <si>
+    <t>Shade Lord Mind Flayer</t>
+  </si>
+  <si>
+    <t>475000-525000</t>
   </si>
 </sst>
 </file>
@@ -406,7 +319,7 @@
   </cellStyleXfs>
   <cellXfs count="1">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +620,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AP27"/>
+  <dimension ref="A1:AP29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,7 +629,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="30" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="32" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="8" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8" bestFit="true" customWidth="true" style="0"/>
@@ -730,17 +643,17 @@
     <col min="13" max="13" width="6" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="15" max="15" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="10" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="11" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="13" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="4" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="5" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="9" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="18" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="16" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="19" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="19" bestFit="true" customWidth="true" style="0"/>
     <col min="29" max="29" width="22" bestFit="true" customWidth="true" style="0"/>
@@ -753,7 +666,7 @@
     <col min="36" max="36" width="21" bestFit="true" customWidth="true" style="0"/>
     <col min="37" max="37" width="17" bestFit="true" customWidth="true" style="0"/>
     <col min="38" max="38" width="22" bestFit="true" customWidth="true" style="0"/>
-    <col min="39" max="39" width="16" bestFit="true" customWidth="true" style="0"/>
+    <col min="39" max="39" width="38" bestFit="true" customWidth="true" style="0"/>
     <col min="40" max="40" width="26" bestFit="true" customWidth="true" style="0"/>
     <col min="41" max="41" width="13" bestFit="true" customWidth="true" style="0"/>
     <col min="42" max="42" width="17" bestFit="true" customWidth="true" style="0"/>
@@ -889,34 +802,34 @@
     </row>
     <row r="2" spans="1:42">
       <c r="A2">
-        <v>64</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="D2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="E2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="F2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="G2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="H2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="I2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>420000</v>
       </c>
       <c r="K2">
         <v>0.5</v>
@@ -934,10 +847,10 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>20000</v>
+        <v>40000</v>
       </c>
       <c r="Q2">
-        <v>2500</v>
+        <v>400</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -946,52 +859,67 @@
         <v>99999</v>
       </c>
       <c r="T2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U2">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="V2">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="W2">
-        <v>89733</v>
+        <v>150000</v>
       </c>
       <c r="X2">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Y2" t="s">
         <v>43</v>
       </c>
       <c r="Z2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA2">
+        <v>95000</v>
+      </c>
+      <c r="AB2">
+        <v>95000</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>0.58</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="s">
         <v>44</v>
       </c>
-      <c r="AA2">
-        <v>70000</v>
-      </c>
-      <c r="AB2">
-        <v>70000</v>
-      </c>
-      <c r="AC2">
-        <v>1</v>
-      </c>
-      <c r="AD2">
-        <v>1</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
-        <v>0.52</v>
-      </c>
-      <c r="AM2">
-        <v>65480</v>
-      </c>
       <c r="AN2">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="AO2">
         <v>1</v>
@@ -999,34 +927,34 @@
     </row>
     <row r="3" spans="1:42">
       <c r="A3">
-        <v>65</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="D3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="E3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="F3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="G3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="H3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="I3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="J3">
-        <v>2300</v>
+        <v>450000</v>
       </c>
       <c r="K3">
         <v>0.5</v>
@@ -1044,10 +972,10 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="Q3">
-        <v>2800</v>
+        <v>450</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -1056,31 +984,31 @@
         <v>99999</v>
       </c>
       <c r="T3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U3">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="V3">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="W3">
-        <v>91365</v>
+        <v>200000</v>
       </c>
       <c r="X3">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="Y3" t="s">
         <v>46</v>
       </c>
       <c r="Z3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AA3">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="AB3">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="AC3">
         <v>1</v>
@@ -1095,13 +1023,22 @@
         <v>1</v>
       </c>
       <c r="AG3">
-        <v>0.55</v>
-      </c>
-      <c r="AM3">
-        <v>65473</v>
-      </c>
-      <c r="AN3">
-        <v>0.01</v>
+        <v>0.6</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
       </c>
       <c r="AO3">
         <v>1</v>
@@ -1109,55 +1046,55 @@
     </row>
     <row r="4" spans="1:42">
       <c r="A4">
-        <v>66</v>
+        <v>341</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="D4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="E4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="F4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="G4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="H4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="I4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="J4">
-        <v>2800</v>
+        <v>460000</v>
       </c>
       <c r="K4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="L4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="M4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="Q4">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -1166,31 +1103,31 @@
         <v>99999</v>
       </c>
       <c r="T4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U4">
-        <v>100</v>
+        <v>193</v>
       </c>
       <c r="V4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="W4">
-        <v>500000</v>
+        <v>225000</v>
       </c>
       <c r="X4">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Y4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AA4">
-        <v>95000</v>
+        <v>120000</v>
       </c>
       <c r="AB4">
-        <v>95000</v>
+        <v>120000</v>
       </c>
       <c r="AC4">
         <v>1</v>
@@ -1205,13 +1142,22 @@
         <v>1</v>
       </c>
       <c r="AG4">
-        <v>0.58</v>
-      </c>
-      <c r="AM4">
-        <v>65473</v>
-      </c>
-      <c r="AN4">
-        <v>0.01</v>
+        <v>0.7</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
       </c>
       <c r="AO4">
         <v>1</v>
@@ -1219,55 +1165,55 @@
     </row>
     <row r="5" spans="1:42">
       <c r="A5">
-        <v>67</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="D5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="E5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="F5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="G5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="H5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="I5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="J5">
-        <v>3186</v>
+        <v>475000</v>
       </c>
       <c r="K5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="M5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="N5">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>100000</v>
+        <v>80000</v>
       </c>
       <c r="Q5">
-        <v>5000</v>
+        <v>550</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -1276,31 +1222,31 @@
         <v>99999</v>
       </c>
       <c r="T5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U5">
-        <v>100</v>
+        <v>229</v>
       </c>
       <c r="V5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="W5">
-        <v>750000</v>
+        <v>250000</v>
       </c>
       <c r="X5">
         <v>24</v>
       </c>
       <c r="Y5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Z5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AA5">
-        <v>300000</v>
+        <v>130000</v>
       </c>
       <c r="AB5">
-        <v>300000</v>
+        <v>130000</v>
       </c>
       <c r="AC5">
         <v>1</v>
@@ -1315,7 +1261,22 @@
         <v>1</v>
       </c>
       <c r="AG5">
-        <v>0.6</v>
+        <v>0.9</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
       </c>
       <c r="AO5">
         <v>1</v>
@@ -1323,55 +1284,55 @@
     </row>
     <row r="6" spans="1:42">
       <c r="A6">
-        <v>241</v>
+        <v>343</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="D6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="E6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="F6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="G6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="H6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="I6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="J6">
-        <v>30000</v>
+        <v>490000</v>
       </c>
       <c r="K6">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="L6">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="M6">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="N6">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="Q6">
-        <v>7000</v>
+        <v>700</v>
       </c>
       <c r="R6">
         <v>1</v>
@@ -1380,31 +1341,31 @@
         <v>99999</v>
       </c>
       <c r="T6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U6">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="V6">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="W6">
-        <v>1000000</v>
+        <v>275000</v>
       </c>
       <c r="X6">
         <v>24</v>
       </c>
       <c r="Y6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Z6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AA6">
-        <v>725000</v>
+        <v>140000</v>
       </c>
       <c r="AB6">
-        <v>725000</v>
+        <v>140000</v>
       </c>
       <c r="AC6">
         <v>1</v>
@@ -1419,7 +1380,22 @@
         <v>1</v>
       </c>
       <c r="AG6">
-        <v>0.7</v>
+        <v>0.95</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
       </c>
       <c r="AO6">
         <v>1</v>
@@ -1427,55 +1403,49 @@
     </row>
     <row r="7" spans="1:42">
       <c r="A7">
-        <v>242</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="D7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="E7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="F7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="G7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="H7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="I7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="J7">
-        <v>40000</v>
+        <v>500000</v>
       </c>
       <c r="K7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>1</v>
-      </c>
-      <c r="P7">
-        <v>500000</v>
-      </c>
-      <c r="Q7">
-        <v>7000</v>
       </c>
       <c r="R7">
         <v>1</v>
@@ -1484,31 +1454,31 @@
         <v>99999</v>
       </c>
       <c r="T7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U7">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="V7">
-        <v>0.05</v>
+        <v>0.75</v>
       </c>
       <c r="W7">
-        <v>10000000</v>
+        <v>350000</v>
       </c>
       <c r="X7">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="Y7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="Z7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AA7">
-        <v>825000</v>
+        <v>150000</v>
       </c>
       <c r="AB7">
-        <v>825000</v>
+        <v>150000</v>
       </c>
       <c r="AC7">
         <v>1</v>
@@ -1523,63 +1493,81 @@
         <v>1</v>
       </c>
       <c r="AG7">
-        <v>0.9</v>
+        <v>0.98</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0.25</v>
+      </c>
+      <c r="AJ7">
+        <v>0.15</v>
+      </c>
+      <c r="AK7">
+        <v>0.15</v>
+      </c>
+      <c r="AL7">
+        <v>0.15</v>
       </c>
       <c r="AO7">
+        <v>1</v>
+      </c>
+      <c r="AP7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:42">
       <c r="A8">
-        <v>243</v>
+        <v>345</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="D8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="E8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="F8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="G8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="H8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="I8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="J8">
-        <v>50000</v>
+        <v>375000</v>
       </c>
       <c r="K8">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="L8">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="M8">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="N8">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="O8">
         <v>1</v>
       </c>
       <c r="P8">
-        <v>1000000</v>
+        <v>10000</v>
       </c>
       <c r="Q8">
-        <v>7000</v>
+        <v>250</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -1588,31 +1576,31 @@
         <v>99999</v>
       </c>
       <c r="T8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="V8">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="W8">
-        <v>100000000</v>
+        <v>50000</v>
       </c>
       <c r="X8">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="Y8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="Z8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="AA8">
-        <v>1200000</v>
+        <v>70000</v>
       </c>
       <c r="AB8">
-        <v>1200000</v>
+        <v>70000</v>
       </c>
       <c r="AC8">
         <v>1</v>
@@ -1627,7 +1615,28 @@
         <v>1</v>
       </c>
       <c r="AG8">
-        <v>0.95</v>
+        <v>0.52</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN8">
+        <v>0.25</v>
       </c>
       <c r="AO8">
         <v>1</v>
@@ -1635,82 +1644,88 @@
     </row>
     <row r="9" spans="1:42">
       <c r="A9">
-        <v>520</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="D9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="E9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="F9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="G9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="H9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="I9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="J9">
-        <v>60000</v>
+        <v>380000</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
+      <c r="P9">
+        <v>20000</v>
+      </c>
+      <c r="Q9">
+        <v>300</v>
+      </c>
       <c r="R9">
         <v>1</v>
       </c>
       <c r="S9">
-        <v>999999</v>
+        <v>99999</v>
       </c>
       <c r="T9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U9">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="V9">
-        <v>0.75</v>
+        <v>0.02</v>
       </c>
       <c r="W9">
-        <v>2000000</v>
+        <v>100000</v>
       </c>
       <c r="X9">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="Y9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="Z9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AA9">
-        <v>150000</v>
+        <v>80000</v>
       </c>
       <c r="AB9">
-        <v>150000</v>
+        <v>80000</v>
       </c>
       <c r="AC9">
         <v>1</v>
@@ -1724,43 +1739,64 @@
       <c r="AF9">
         <v>1</v>
       </c>
+      <c r="AG9">
+        <v>0.55</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN9">
+        <v>0.01</v>
+      </c>
       <c r="AO9">
-        <v>1</v>
-      </c>
-      <c r="AP9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:42">
       <c r="A10">
-        <v>68</v>
+        <v>352</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="D10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="E10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="F10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="G10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="H10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="I10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="J10">
-        <v>70000</v>
+        <v>200000</v>
       </c>
       <c r="K10">
         <v>0.6</v>
@@ -1778,10 +1814,10 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>40000</v>
+        <v>70000</v>
       </c>
       <c r="Q10">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -1790,31 +1826,31 @@
         <v>99999</v>
       </c>
       <c r="T10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U10">
-        <v>100</v>
+        <v>264</v>
       </c>
       <c r="V10">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="W10">
-        <v>100000000</v>
+        <v>225000</v>
       </c>
       <c r="X10">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Y10" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="Z10" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="AA10">
-        <v>650000</v>
+        <v>120000</v>
       </c>
       <c r="AB10">
-        <v>650000</v>
+        <v>120000</v>
       </c>
       <c r="AC10">
         <v>1</v>
@@ -1829,7 +1865,22 @@
         <v>1</v>
       </c>
       <c r="AG10">
-        <v>0.55</v>
+        <v>0.7</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
       </c>
       <c r="AO10">
         <v>2</v>
@@ -1837,34 +1888,34 @@
     </row>
     <row r="11" spans="1:42">
       <c r="A11">
-        <v>69</v>
+        <v>356</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="D11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="E11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="F11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="G11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="H11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="I11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="J11">
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="K11">
         <v>0.6</v>
@@ -1882,10 +1933,10 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>80000</v>
+        <v>10000</v>
       </c>
       <c r="Q11">
-        <v>2800</v>
+        <v>250</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -1894,31 +1945,31 @@
         <v>99999</v>
       </c>
       <c r="T11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U11">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="V11">
-        <v>0.01</v>
+        <v>0.15</v>
       </c>
       <c r="W11">
-        <v>200000000</v>
+        <v>50000</v>
       </c>
       <c r="X11">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="Y11" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="Z11" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="AA11">
-        <v>800000</v>
+        <v>70000</v>
       </c>
       <c r="AB11">
-        <v>800000</v>
+        <v>70000</v>
       </c>
       <c r="AC11">
         <v>1</v>
@@ -1933,7 +1984,22 @@
         <v>1</v>
       </c>
       <c r="AG11">
-        <v>0.58</v>
+        <v>0.55</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
       </c>
       <c r="AO11">
         <v>2</v>
@@ -1941,34 +2007,34 @@
     </row>
     <row r="12" spans="1:42">
       <c r="A12">
-        <v>70</v>
+        <v>355</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="D12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="E12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="F12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="G12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="H12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="I12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="J12">
-        <v>95000</v>
+        <v>80000</v>
       </c>
       <c r="K12">
         <v>0.6</v>
@@ -1986,10 +2052,10 @@
         <v>1</v>
       </c>
       <c r="P12">
-        <v>160000</v>
+        <v>20000</v>
       </c>
       <c r="Q12">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -1998,31 +2064,31 @@
         <v>99999</v>
       </c>
       <c r="T12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U12">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="V12">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="W12">
-        <v>350000000</v>
+        <v>100000</v>
       </c>
       <c r="X12">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="Y12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="Z12" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="AA12">
-        <v>950000</v>
+        <v>80000</v>
       </c>
       <c r="AB12">
-        <v>950000</v>
+        <v>80000</v>
       </c>
       <c r="AC12">
         <v>1</v>
@@ -2037,13 +2103,22 @@
         <v>1</v>
       </c>
       <c r="AG12">
-        <v>0.6</v>
-      </c>
-      <c r="AM12">
-        <v>65469</v>
-      </c>
-      <c r="AN12">
-        <v>0.2</v>
+        <v>0.58</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
       </c>
       <c r="AO12">
         <v>2</v>
@@ -2051,34 +2126,34 @@
     </row>
     <row r="13" spans="1:42">
       <c r="A13">
-        <v>71</v>
+        <v>354</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="D13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="E13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="F13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="G13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="H13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="I13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="J13">
-        <v>100000</v>
+        <v>95000</v>
       </c>
       <c r="K13">
         <v>0.6</v>
@@ -2096,10 +2171,10 @@
         <v>1</v>
       </c>
       <c r="P13">
-        <v>220000</v>
+        <v>40000</v>
       </c>
       <c r="Q13">
-        <v>5000</v>
+        <v>400</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -2108,31 +2183,31 @@
         <v>99999</v>
       </c>
       <c r="T13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U13">
-        <v>100</v>
+        <v>169</v>
       </c>
       <c r="V13">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="W13">
-        <v>500000000</v>
+        <v>150000</v>
       </c>
       <c r="X13">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Y13" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="Z13" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="AA13">
-        <v>1100000</v>
+        <v>95000</v>
       </c>
       <c r="AB13">
-        <v>1100000</v>
+        <v>95000</v>
       </c>
       <c r="AC13">
         <v>1</v>
@@ -2147,7 +2222,28 @@
         <v>1</v>
       </c>
       <c r="AG13">
-        <v>0.65</v>
+        <v>0.6</v>
+      </c>
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <v>0</v>
+      </c>
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN13">
+        <v>0.2</v>
       </c>
       <c r="AO13">
         <v>2</v>
@@ -2155,34 +2251,34 @@
     </row>
     <row r="14" spans="1:42">
       <c r="A14">
-        <v>72</v>
+        <v>353</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="D14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="E14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="F14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="G14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="H14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="I14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="J14">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="K14">
         <v>0.6</v>
@@ -2200,10 +2296,10 @@
         <v>1</v>
       </c>
       <c r="P14">
-        <v>440000</v>
+        <v>60000</v>
       </c>
       <c r="Q14">
-        <v>8000</v>
+        <v>450</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -2212,31 +2308,31 @@
         <v>99999</v>
       </c>
       <c r="T14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U14">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="V14">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="W14">
-        <v>1000000000</v>
+        <v>200000</v>
       </c>
       <c r="X14">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Y14" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="Z14" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="AA14">
-        <v>1400000</v>
+        <v>100000</v>
       </c>
       <c r="AB14">
-        <v>1400000</v>
+        <v>100000</v>
       </c>
       <c r="AC14">
         <v>1</v>
@@ -2251,7 +2347,22 @@
         <v>1</v>
       </c>
       <c r="AG14">
-        <v>0.7</v>
+        <v>0.65</v>
+      </c>
+      <c r="AH14">
+        <v>0</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
       </c>
       <c r="AO14">
         <v>2</v>
@@ -2259,10 +2370,10 @@
     </row>
     <row r="15" spans="1:42">
       <c r="A15">
-        <v>244</v>
+        <v>351</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <v>225000</v>
@@ -2304,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="P15">
-        <v>1000000</v>
+        <v>80000</v>
       </c>
       <c r="Q15">
-        <v>9000</v>
+        <v>550</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -2319,28 +2430,28 @@
         <v>3</v>
       </c>
       <c r="U15">
-        <v>100</v>
+        <v>311</v>
       </c>
       <c r="V15">
         <v>0.15</v>
       </c>
       <c r="W15">
-        <v>1000000000</v>
+        <v>250000</v>
       </c>
       <c r="X15">
         <v>36</v>
       </c>
       <c r="Y15" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="Z15" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="AA15">
-        <v>1800000</v>
+        <v>130000</v>
       </c>
       <c r="AB15">
-        <v>1800000</v>
+        <v>130000</v>
       </c>
       <c r="AC15">
         <v>1</v>
@@ -2356,6 +2467,21 @@
       </c>
       <c r="AG15">
         <v>0.8</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <v>0</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
       </c>
       <c r="AO15">
         <v>2</v>
@@ -2363,55 +2489,55 @@
     </row>
     <row r="16" spans="1:42">
       <c r="A16">
-        <v>245</v>
+        <v>350</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="D16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="E16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="F16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="G16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="H16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="I16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="J16">
-        <v>250000</v>
+        <v>280000</v>
       </c>
       <c r="K16">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="L16">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="M16">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="N16">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16">
-        <v>5000000</v>
+        <v>10000</v>
       </c>
       <c r="Q16">
-        <v>10000</v>
+        <v>250</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -2420,31 +2546,31 @@
         <v>99999</v>
       </c>
       <c r="T16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U16">
-        <v>100</v>
+        <v>406</v>
       </c>
       <c r="V16">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="W16">
-        <v>1000000000</v>
+        <v>50000</v>
       </c>
       <c r="X16">
         <v>40</v>
       </c>
       <c r="Y16" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="Z16" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="AA16">
-        <v>2200000</v>
+        <v>70000</v>
       </c>
       <c r="AB16">
-        <v>2200000</v>
+        <v>70000</v>
       </c>
       <c r="AC16">
         <v>1</v>
@@ -2459,7 +2585,22 @@
         <v>1</v>
       </c>
       <c r="AG16">
-        <v>0.85</v>
+        <v>0.9</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
       </c>
       <c r="AO16">
         <v>2</v>
@@ -2467,55 +2608,55 @@
     </row>
     <row r="17" spans="1:42">
       <c r="A17">
-        <v>246</v>
+        <v>349</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="D17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="E17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="F17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="G17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="H17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="I17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="J17">
-        <v>280000</v>
+        <v>300000</v>
       </c>
       <c r="K17">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="L17">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="M17">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="N17">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17">
-        <v>8000000</v>
+        <v>20000</v>
       </c>
       <c r="Q17">
-        <v>11000</v>
+        <v>300</v>
       </c>
       <c r="R17">
         <v>1</v>
@@ -2524,31 +2665,31 @@
         <v>99999</v>
       </c>
       <c r="T17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U17">
-        <v>100</v>
+        <v>453</v>
       </c>
       <c r="V17">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="W17">
-        <v>2000000000</v>
+        <v>100000</v>
       </c>
       <c r="X17">
         <v>40</v>
       </c>
       <c r="Y17" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="Z17" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="AA17">
-        <v>2500000</v>
+        <v>80000</v>
       </c>
       <c r="AB17">
-        <v>2500000</v>
+        <v>80000</v>
       </c>
       <c r="AC17">
         <v>1</v>
@@ -2564,6 +2705,21 @@
       </c>
       <c r="AG17">
         <v>0.9</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
       </c>
       <c r="AO17">
         <v>2</v>
@@ -2571,55 +2727,55 @@
     </row>
     <row r="18" spans="1:42">
       <c r="A18">
-        <v>247</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="C18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="D18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="E18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="F18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="G18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="H18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="I18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="J18">
-        <v>300000</v>
+        <v>325000</v>
       </c>
       <c r="K18">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="L18">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="M18">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="N18">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="P18">
-        <v>10000000</v>
+        <v>40000</v>
       </c>
       <c r="Q18">
-        <v>12000</v>
+        <v>400</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -2628,31 +2784,31 @@
         <v>99999</v>
       </c>
       <c r="T18" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U18">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="V18">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="W18">
-        <v>2000000000</v>
+        <v>150000</v>
       </c>
       <c r="X18">
         <v>40</v>
       </c>
       <c r="Y18" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="Z18" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="AA18">
-        <v>2800000</v>
+        <v>95000</v>
       </c>
       <c r="AB18">
-        <v>2800000</v>
+        <v>95000</v>
       </c>
       <c r="AC18">
         <v>1</v>
@@ -2668,6 +2824,21 @@
       </c>
       <c r="AG18">
         <v>0.9</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
       </c>
       <c r="AO18">
         <v>2</v>
@@ -2675,55 +2846,49 @@
     </row>
     <row r="19" spans="1:42">
       <c r="A19">
-        <v>248</v>
+        <v>347</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="D19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="E19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="F19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="G19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="H19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="I19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="J19">
-        <v>325000</v>
+        <v>600000</v>
       </c>
       <c r="K19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="M19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <v>1</v>
-      </c>
-      <c r="P19">
-        <v>12000000</v>
-      </c>
-      <c r="Q19">
-        <v>13000</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2732,31 +2897,31 @@
         <v>99999</v>
       </c>
       <c r="T19" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="U19">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="V19">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="W19">
-        <v>2000000000</v>
+        <v>500000</v>
       </c>
       <c r="X19">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="Y19" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="Z19" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="AA19">
-        <v>3200000</v>
+        <v>300000</v>
       </c>
       <c r="AB19">
-        <v>3200000</v>
+        <v>300000</v>
       </c>
       <c r="AC19">
         <v>1</v>
@@ -2771,63 +2936,84 @@
         <v>1</v>
       </c>
       <c r="AG19">
-        <v>0.9</v>
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>1</v>
+      </c>
+      <c r="AI19">
+        <v>0.3</v>
+      </c>
+      <c r="AJ19">
+        <v>0.3</v>
+      </c>
+      <c r="AK19">
+        <v>0.3</v>
+      </c>
+      <c r="AL19">
+        <v>0.3</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
       </c>
       <c r="AO19">
         <v>2</v>
+      </c>
+      <c r="AP19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:42">
       <c r="A20">
-        <v>106</v>
+        <v>346</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="D20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="E20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="F20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="G20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="H20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="I20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="J20">
-        <v>350000</v>
+        <v>250000</v>
       </c>
       <c r="K20">
-        <v>0.98</v>
+        <v>0.7</v>
       </c>
       <c r="L20">
-        <v>0.98</v>
+        <v>0.7</v>
       </c>
       <c r="M20">
-        <v>0.98</v>
+        <v>0.7</v>
       </c>
       <c r="N20">
-        <v>0.98</v>
+        <v>0.7</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
       <c r="P20">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="Q20">
-        <v>5000</v>
+        <v>700</v>
       </c>
       <c r="R20">
         <v>1</v>
@@ -2836,31 +3022,31 @@
         <v>99999</v>
       </c>
       <c r="T20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U20">
-        <v>100</v>
+        <v>358</v>
       </c>
       <c r="V20">
         <v>0.01</v>
       </c>
       <c r="W20">
-        <v>10000000</v>
+        <v>275000</v>
       </c>
       <c r="X20">
         <v>40</v>
       </c>
       <c r="Y20" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="Z20" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="AA20">
-        <v>2800000</v>
+        <v>140000</v>
       </c>
       <c r="AB20">
-        <v>2800000</v>
+        <v>140000</v>
       </c>
       <c r="AC20">
         <v>1</v>
@@ -2875,42 +3061,57 @@
         <v>1</v>
       </c>
       <c r="AG20">
-        <v>0.8</v>
+        <v>0.85</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
       </c>
       <c r="AO20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:42">
       <c r="A21">
-        <v>107</v>
+        <v>357</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="C21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="D21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="E21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="F21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="G21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="H21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="I21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="J21">
-        <v>370000</v>
+        <v>350000</v>
       </c>
       <c r="K21">
         <v>0.98</v>
@@ -2928,10 +3129,10 @@
         <v>1</v>
       </c>
       <c r="P21">
-        <v>1000000</v>
+        <v>60000</v>
       </c>
       <c r="Q21">
-        <v>8000</v>
+        <v>450</v>
       </c>
       <c r="R21">
         <v>1</v>
@@ -2940,31 +3141,31 @@
         <v>99999</v>
       </c>
       <c r="T21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U21">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="V21">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="W21">
-        <v>15000000</v>
+        <v>200000</v>
       </c>
       <c r="X21">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Y21" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="Z21" t="s">
-        <v>100</v>
+        <v>46</v>
       </c>
       <c r="AA21">
-        <v>3200000</v>
+        <v>100000</v>
       </c>
       <c r="AB21">
-        <v>3200000</v>
+        <v>100000</v>
       </c>
       <c r="AC21">
         <v>1</v>
@@ -2979,7 +3180,22 @@
         <v>1</v>
       </c>
       <c r="AG21">
-        <v>0.85</v>
+        <v>0.8</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
       </c>
       <c r="AO21">
         <v>3</v>
@@ -2987,34 +3203,34 @@
     </row>
     <row r="22" spans="1:42">
       <c r="A22">
-        <v>108</v>
+        <v>358</v>
       </c>
       <c r="B22" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="D22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="E22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="F22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="G22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="H22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="I22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="J22">
-        <v>450000</v>
+        <v>370000</v>
       </c>
       <c r="K22">
         <v>0.98</v>
@@ -3032,10 +3248,10 @@
         <v>1</v>
       </c>
       <c r="P22">
-        <v>5000000</v>
+        <v>70000</v>
       </c>
       <c r="Q22">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="R22">
         <v>1</v>
@@ -3044,31 +3260,31 @@
         <v>99999</v>
       </c>
       <c r="T22" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U22">
-        <v>100</v>
+        <v>833</v>
       </c>
       <c r="V22">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="W22">
-        <v>30000000</v>
+        <v>225000</v>
       </c>
       <c r="X22">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Y22" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
       <c r="Z22" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="AA22">
-        <v>3800000</v>
+        <v>120000</v>
       </c>
       <c r="AB22">
-        <v>3800000</v>
+        <v>120000</v>
       </c>
       <c r="AC22">
         <v>1</v>
@@ -3083,7 +3299,22 @@
         <v>1</v>
       </c>
       <c r="AG22">
-        <v>0.9</v>
+        <v>0.85</v>
+      </c>
+      <c r="AH22">
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
       </c>
       <c r="AO22">
         <v>3</v>
@@ -3091,34 +3322,34 @@
     </row>
     <row r="23" spans="1:42">
       <c r="A23">
-        <v>109</v>
+        <v>359</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="D23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="E23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="F23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="G23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="H23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="I23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="J23">
-        <v>500000</v>
+        <v>450000</v>
       </c>
       <c r="K23">
         <v>0.98</v>
@@ -3136,10 +3367,10 @@
         <v>1</v>
       </c>
       <c r="P23">
-        <v>100000000</v>
+        <v>80000</v>
       </c>
       <c r="Q23">
-        <v>24000</v>
+        <v>550</v>
       </c>
       <c r="R23">
         <v>1</v>
@@ -3148,31 +3379,31 @@
         <v>99999</v>
       </c>
       <c r="T23" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U23">
-        <v>100</v>
+        <v>967</v>
       </c>
       <c r="V23">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="W23">
-        <v>2000000000</v>
+        <v>250000</v>
       </c>
       <c r="X23">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="Y23" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="Z23" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="AA23">
-        <v>4000000</v>
+        <v>130000</v>
       </c>
       <c r="AB23">
-        <v>4000000</v>
+        <v>130000</v>
       </c>
       <c r="AC23">
         <v>1</v>
@@ -3187,7 +3418,22 @@
         <v>1</v>
       </c>
       <c r="AG23">
-        <v>1</v>
+        <v>0.9</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
       </c>
       <c r="AO23">
         <v>3</v>
@@ -3195,34 +3441,34 @@
     </row>
     <row r="24" spans="1:42">
       <c r="A24">
-        <v>110</v>
+        <v>360</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="D24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="E24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="F24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="G24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="H24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="I24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="J24">
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="K24">
         <v>0.98</v>
@@ -3240,10 +3486,10 @@
         <v>1</v>
       </c>
       <c r="P24">
-        <v>100000000</v>
+        <v>100000</v>
       </c>
       <c r="Q24">
-        <v>24000</v>
+        <v>700</v>
       </c>
       <c r="R24">
         <v>1</v>
@@ -3252,31 +3498,31 @@
         <v>99999</v>
       </c>
       <c r="T24" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U24">
-        <v>100</v>
+        <v>1100</v>
       </c>
       <c r="V24">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="W24">
-        <v>2000000000</v>
+        <v>275000</v>
       </c>
       <c r="X24">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="Y24" t="s">
-        <v>108</v>
+        <v>52</v>
       </c>
       <c r="Z24" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="AA24">
-        <v>4200000</v>
+        <v>140000</v>
       </c>
       <c r="AB24">
-        <v>4200000</v>
+        <v>140000</v>
       </c>
       <c r="AC24">
         <v>1</v>
@@ -3292,6 +3538,21 @@
       </c>
       <c r="AG24">
         <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
       </c>
       <c r="AO24">
         <v>3</v>
@@ -3299,34 +3560,34 @@
     </row>
     <row r="25" spans="1:42">
       <c r="A25">
-        <v>265</v>
+        <v>361</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="D25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="E25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="F25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="G25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="H25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="I25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="J25">
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="K25">
         <v>0.98</v>
@@ -3344,10 +3605,10 @@
         <v>1</v>
       </c>
       <c r="P25">
-        <v>100000000</v>
+        <v>500000</v>
       </c>
       <c r="Q25">
-        <v>24000</v>
+        <v>1000</v>
       </c>
       <c r="R25">
         <v>1</v>
@@ -3359,28 +3620,28 @@
         <v>3</v>
       </c>
       <c r="U25">
+        <v>1233</v>
+      </c>
+      <c r="V25">
+        <v>0.15</v>
+      </c>
+      <c r="W25">
+        <v>300000</v>
+      </c>
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="V25">
-        <v>0.05</v>
-      </c>
-      <c r="W25">
-        <v>2000000000</v>
-      </c>
-      <c r="X25">
-        <v>120</v>
-      </c>
       <c r="Y25" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="Z25" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="AA25">
-        <v>4800000</v>
+        <v>150000</v>
       </c>
       <c r="AB25">
-        <v>4800000</v>
+        <v>150000</v>
       </c>
       <c r="AC25">
         <v>1</v>
@@ -3396,6 +3657,21 @@
       </c>
       <c r="AG25">
         <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>0</v>
+      </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>0</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>0</v>
       </c>
       <c r="AO25">
         <v>3</v>
@@ -3403,55 +3679,49 @@
     </row>
     <row r="26" spans="1:42">
       <c r="A26">
-        <v>307</v>
+        <v>362</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="D26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="E26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="F26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="G26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="H26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="I26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="J26">
-        <v>800000</v>
+        <v>625000</v>
       </c>
       <c r="K26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O26">
         <v>1</v>
-      </c>
-      <c r="P26">
-        <v>1000000000</v>
-      </c>
-      <c r="Q26">
-        <v>5000</v>
       </c>
       <c r="R26">
         <v>1</v>
@@ -3460,87 +3730,102 @@
         <v>99999</v>
       </c>
       <c r="T26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="U26">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="V26">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="W26">
-        <v>2000000000</v>
+        <v>600000</v>
       </c>
       <c r="X26">
-        <v>200</v>
+        <v>125</v>
       </c>
       <c r="Y26" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="Z26" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="AA26">
-        <v>8000000</v>
+        <v>400000</v>
       </c>
       <c r="AB26">
-        <v>8000000</v>
+        <v>400000</v>
       </c>
       <c r="AC26">
         <v>1</v>
       </c>
       <c r="AD26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AE26">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AF26">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AG26">
-        <v>0.75</v>
-      </c>
-      <c r="AM26">
-        <v>296287</v>
+        <v>1</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0.4</v>
+      </c>
+      <c r="AJ26">
+        <v>0.4</v>
+      </c>
+      <c r="AK26">
+        <v>0.4</v>
+      </c>
+      <c r="AL26">
+        <v>0.4</v>
       </c>
       <c r="AN26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO26">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="AP26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:42">
       <c r="A27">
-        <v>401</v>
+        <v>363</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="C27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="D27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="E27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="F27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="G27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="H27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="I27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="J27">
-        <v>850000</v>
+        <v>800000</v>
       </c>
       <c r="K27">
         <v>2</v>
@@ -3558,10 +3843,10 @@
         <v>1</v>
       </c>
       <c r="P27">
-        <v>2000000000</v>
+        <v>25000</v>
       </c>
       <c r="Q27">
-        <v>10000</v>
+        <v>300</v>
       </c>
       <c r="R27">
         <v>1</v>
@@ -3570,52 +3855,64 @@
         <v>99999</v>
       </c>
       <c r="T27" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U27">
-        <v>100</v>
+        <v>1367</v>
       </c>
       <c r="V27">
-        <v>0.01</v>
+        <v>0.25</v>
       </c>
       <c r="W27">
-        <v>2000000000</v>
+        <v>500000</v>
       </c>
       <c r="X27">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="Y27" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="Z27" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="AA27">
-        <v>15000000</v>
+        <v>250000</v>
       </c>
       <c r="AB27">
-        <v>15000000</v>
+        <v>250000</v>
       </c>
       <c r="AC27">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="AD27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF27">
-        <v>1.6</v>
+        <v>0.75</v>
       </c>
       <c r="AG27">
-        <v>1.6</v>
+        <v>0.75</v>
       </c>
       <c r="AH27">
-        <v>1.1517</v>
-      </c>
-      <c r="AM27">
-        <v>308682</v>
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>83</v>
       </c>
       <c r="AN27">
         <v>1</v>
@@ -3624,8 +3921,251 @@
         <v>4</v>
       </c>
     </row>
+    <row r="28" spans="1:42">
+      <c r="A28">
+        <v>364</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28">
+        <v>850000</v>
+      </c>
+      <c r="D28">
+        <v>850000</v>
+      </c>
+      <c r="E28">
+        <v>850000</v>
+      </c>
+      <c r="F28">
+        <v>850000</v>
+      </c>
+      <c r="G28">
+        <v>850000</v>
+      </c>
+      <c r="H28">
+        <v>850000</v>
+      </c>
+      <c r="I28">
+        <v>850000</v>
+      </c>
+      <c r="J28">
+        <v>850000</v>
+      </c>
+      <c r="K28">
+        <v>2</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>350000</v>
+      </c>
+      <c r="Q28">
+        <v>400</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>99999</v>
+      </c>
+      <c r="T28" t="s">
+        <v>4</v>
+      </c>
+      <c r="U28">
+        <v>1500</v>
+      </c>
+      <c r="V28">
+        <v>0.01</v>
+      </c>
+      <c r="W28">
+        <v>1000000</v>
+      </c>
+      <c r="X28">
+        <v>400</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA28">
+        <v>275000</v>
+      </c>
+      <c r="AB28">
+        <v>275000</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
+        <v>1</v>
+      </c>
+      <c r="AE28">
+        <v>1</v>
+      </c>
+      <c r="AF28">
+        <v>1</v>
+      </c>
+      <c r="AG28">
+        <v>1</v>
+      </c>
+      <c r="AH28">
+        <v>1</v>
+      </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AJ28">
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
+      </c>
+      <c r="AM28" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN28">
+        <v>1</v>
+      </c>
+      <c r="AO28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42">
+      <c r="A29">
+        <v>365</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29">
+        <v>650000</v>
+      </c>
+      <c r="D29">
+        <v>650000</v>
+      </c>
+      <c r="E29">
+        <v>650000</v>
+      </c>
+      <c r="F29">
+        <v>650000</v>
+      </c>
+      <c r="G29">
+        <v>650000</v>
+      </c>
+      <c r="H29">
+        <v>650000</v>
+      </c>
+      <c r="I29">
+        <v>650000</v>
+      </c>
+      <c r="J29">
+        <v>650000</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+      <c r="S29">
+        <v>99999</v>
+      </c>
+      <c r="T29" t="s">
+        <v>6</v>
+      </c>
+      <c r="U29">
+        <v>300</v>
+      </c>
+      <c r="V29">
+        <v>0.75</v>
+      </c>
+      <c r="W29">
+        <v>700000</v>
+      </c>
+      <c r="X29">
+        <v>500</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA29">
+        <v>450000</v>
+      </c>
+      <c r="AB29">
+        <v>450000</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>1</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>1</v>
+      </c>
+      <c r="AH29">
+        <v>1</v>
+      </c>
+      <c r="AI29">
+        <v>0.5</v>
+      </c>
+      <c r="AJ29">
+        <v>0.5</v>
+      </c>
+      <c r="AK29">
+        <v>0.5</v>
+      </c>
+      <c r="AL29">
+        <v>0.5</v>
+      </c>
+      <c r="AN29">
+        <v>0</v>
+      </c>
+      <c r="AO29">
+        <v>4</v>
+      </c>
+      <c r="AP29">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>